<commit_message>
corretto documento come indicato via mail
29: È necessario valorizzare la colonna J con 'SI' o 'NO', valorizzare anche le colonne dipendenti dall' applicabilità
37: È necessario valorizzare la colonna J con 'SI' o 'NO', valorizzare anche le colonne dipendenti dall' applicabilità
66: È necessario valorizzare le seguenti colonne: F, G, H, I, L, M, O, P
67: È necessario valorizzare le seguenti colonne: F, G, H, I, L, M, O, P
69: È necessario valorizzare le seguenti colonne: F, G, H, I, L, M, O, P
70: È necessario valorizzare le seguenti colonne: F, G, H, I, L, M, O,
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111HITECHSPAXX/Hi.Tech/AcceWeb/2.1.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111HITECHSPAXX/Hi.Tech/AcceWeb/2.1.0/report-checklist.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="200">
   <si>
     <t xml:space="preserve">COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -231,6 +231,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Hi.Tech</t>
     </r>
@@ -462,6 +463,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Il campo viene sempre valorizzato in automatico dal sistema essendo un campo non gestito dall’utente ma recuperato da configurazioni applicative</t>
+  </si>
+  <si>
     <t xml:space="preserve">KO</t>
   </si>
   <si>
@@ -639,6 +643,9 @@
   </si>
   <si>
     <t xml:space="preserve">Errore semantico.[ERRORE-b5| Sezione Condizioni del paziente e diagnosi alla dimissione: la sezione DEVE essere presente],[ERRORE-b6| Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione DEVE contenere l'elemento 'text'],[W003|  Sezione Condizioni del paziente e diagnosi alla dimissione: La sezione PUO' contenere l'elemento 'entry' ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L’operatore inserisci i dati mancanti ed effettua una nuova validazione</t>
   </si>
   <si>
     <t xml:space="preserve">VALIDAZIONE_CDA2_LDO_CT12_KO</t>
@@ -905,7 +912,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -958,13 +965,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -1187,7 +1187,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1195,11 +1195,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1259,11 +1259,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1383,13 +1383,13 @@
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="J15:J376 A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="130.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="2" style="0" width="8.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="248.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="3" style="0" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2457,10 +2457,10 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J15:J376 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="194.14"/>
@@ -3565,11 +3565,13 @@
   </sheetPr>
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B7" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topRight" activeCell="J15" activeCellId="0" sqref="J15:J376"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.86"/>
@@ -4507,8 +4509,12 @@
       <c r="G36" s="29"/>
       <c r="H36" s="29"/>
       <c r="I36" s="29"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
+      <c r="J36" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="K36" s="35" t="s">
+        <v>78</v>
+      </c>
       <c r="L36" s="30"/>
       <c r="M36" s="30"/>
       <c r="N36" s="30"/>
@@ -4518,7 +4524,7 @@
       <c r="R36" s="31"/>
       <c r="S36" s="32"/>
       <c r="T36" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4686,17 +4692,21 @@
         <v>49</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E44" s="34" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="F44" s="28"/>
       <c r="G44" s="29"/>
       <c r="H44" s="29"/>
       <c r="I44" s="29"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="30"/>
+      <c r="J44" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="K44" s="35" t="s">
+        <v>78</v>
+      </c>
       <c r="L44" s="30"/>
       <c r="M44" s="30"/>
       <c r="N44" s="30"/>
@@ -4706,7 +4716,7 @@
       <c r="R44" s="31"/>
       <c r="S44" s="32"/>
       <c r="T44" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4874,10 +4884,10 @@
         <v>49</v>
       </c>
       <c r="D52" s="26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E52" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F52" s="28" t="n">
         <v>45320</v>
@@ -4885,30 +4895,32 @@
       <c r="G52" s="29"/>
       <c r="H52" s="29"/>
       <c r="I52" s="29"/>
-      <c r="J52" s="30"/>
+      <c r="J52" s="30" t="s">
+        <v>84</v>
+      </c>
       <c r="K52" s="30"/>
       <c r="L52" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M52" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="N52" s="35" t="s">
         <v>84</v>
       </c>
+      <c r="N52" s="30" t="s">
+        <v>85</v>
+      </c>
       <c r="O52" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="P52" s="35" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="P52" s="30" t="s">
+        <v>86</v>
       </c>
       <c r="Q52" s="30"/>
       <c r="R52" s="31" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="S52" s="32"/>
       <c r="T52" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5296,10 +5308,10 @@
         <v>49</v>
       </c>
       <c r="D70" s="26" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E70" s="27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F70" s="28"/>
       <c r="G70" s="29"/>
@@ -5309,7 +5321,7 @@
         <v>55</v>
       </c>
       <c r="K70" s="30" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L70" s="30"/>
       <c r="M70" s="30"/>
@@ -5320,7 +5332,7 @@
       <c r="R70" s="31"/>
       <c r="S70" s="32"/>
       <c r="T70" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5334,10 +5346,10 @@
         <v>49</v>
       </c>
       <c r="D71" s="26" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E71" s="27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F71" s="28"/>
       <c r="G71" s="29"/>
@@ -5347,7 +5359,7 @@
         <v>55</v>
       </c>
       <c r="K71" s="30" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="L71" s="30"/>
       <c r="M71" s="30"/>
@@ -5358,7 +5370,7 @@
       <c r="R71" s="31"/>
       <c r="S71" s="32"/>
       <c r="T71" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5372,10 +5384,10 @@
         <v>49</v>
       </c>
       <c r="D72" s="26" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E72" s="27" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F72" s="28"/>
       <c r="G72" s="29"/>
@@ -5385,7 +5397,7 @@
         <v>55</v>
       </c>
       <c r="K72" s="30" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="L72" s="30"/>
       <c r="M72" s="30"/>
@@ -5396,7 +5408,7 @@
       <c r="R72" s="31"/>
       <c r="S72" s="32"/>
       <c r="T72" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5410,45 +5422,47 @@
         <v>49</v>
       </c>
       <c r="D73" s="26" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E73" s="27" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F73" s="28" t="n">
         <v>45320</v>
       </c>
       <c r="G73" s="29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H73" s="29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="I73" s="29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J73" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K73" s="30"/>
       <c r="L73" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M73" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N73" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="O73" s="30"/>
+        <v>101</v>
+      </c>
+      <c r="O73" s="30" t="s">
+        <v>55</v>
+      </c>
       <c r="P73" s="30" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Q73" s="30"/>
       <c r="R73" s="31"/>
       <c r="S73" s="32"/>
       <c r="T73" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5462,45 +5476,47 @@
         <v>49</v>
       </c>
       <c r="D74" s="26" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E74" s="27" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F74" s="28" t="n">
         <v>45320</v>
       </c>
       <c r="G74" s="29" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H74" s="29" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I74" s="29" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J74" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K74" s="30"/>
       <c r="L74" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M74" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N74" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="O74" s="30"/>
+        <v>108</v>
+      </c>
+      <c r="O74" s="30" t="s">
+        <v>55</v>
+      </c>
       <c r="P74" s="30" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="Q74" s="30"/>
       <c r="R74" s="31"/>
       <c r="S74" s="32"/>
       <c r="T74" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5514,10 +5530,10 @@
         <v>49</v>
       </c>
       <c r="D75" s="26" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E75" s="27" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F75" s="28"/>
       <c r="G75" s="29"/>
@@ -5527,7 +5543,7 @@
         <v>55</v>
       </c>
       <c r="K75" s="30" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L75" s="30"/>
       <c r="M75" s="30"/>
@@ -5538,7 +5554,7 @@
       <c r="R75" s="31"/>
       <c r="S75" s="32"/>
       <c r="T75" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5552,43 +5568,47 @@
         <v>49</v>
       </c>
       <c r="D76" s="26" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E76" s="27" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F76" s="28" t="n">
         <v>45320</v>
       </c>
       <c r="G76" s="29" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H76" s="29" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I76" s="29" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J76" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K76" s="30"/>
       <c r="L76" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M76" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N76" s="30" t="s">
-        <v>116</v>
-      </c>
-      <c r="O76" s="30"/>
-      <c r="P76" s="30"/>
+        <v>117</v>
+      </c>
+      <c r="O76" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="P76" s="35" t="s">
+        <v>118</v>
+      </c>
       <c r="Q76" s="30"/>
       <c r="R76" s="31"/>
       <c r="S76" s="32"/>
       <c r="T76" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5602,43 +5622,47 @@
         <v>49</v>
       </c>
       <c r="D77" s="26" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E77" s="27" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F77" s="28" t="n">
         <v>45320</v>
       </c>
       <c r="G77" s="29" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H77" s="29" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="I77" s="29" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="J77" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K77" s="30"/>
       <c r="L77" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="M77" s="30" t="s">
-        <v>83</v>
-      </c>
-      <c r="N77" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="O77" s="30"/>
-      <c r="P77" s="30"/>
+        <v>84</v>
+      </c>
+      <c r="N77" s="30" t="s">
+        <v>124</v>
+      </c>
+      <c r="O77" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="P77" s="35" t="s">
+        <v>118</v>
+      </c>
       <c r="Q77" s="30"/>
       <c r="R77" s="31"/>
       <c r="S77" s="32"/>
       <c r="T77" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5652,10 +5676,10 @@
         <v>49</v>
       </c>
       <c r="D78" s="26" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E78" s="27" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F78" s="28"/>
       <c r="G78" s="29"/>
@@ -5665,7 +5689,7 @@
         <v>55</v>
       </c>
       <c r="K78" s="30" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="L78" s="30"/>
       <c r="M78" s="30"/>
@@ -5676,7 +5700,7 @@
       <c r="R78" s="31"/>
       <c r="S78" s="32"/>
       <c r="T78" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5690,10 +5714,10 @@
         <v>49</v>
       </c>
       <c r="D79" s="26" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E79" s="27" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F79" s="28"/>
       <c r="G79" s="29"/>
@@ -5703,7 +5727,7 @@
         <v>55</v>
       </c>
       <c r="K79" s="30" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L79" s="30"/>
       <c r="M79" s="30"/>
@@ -5714,7 +5738,7 @@
       <c r="R79" s="31"/>
       <c r="S79" s="32"/>
       <c r="T79" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5728,10 +5752,10 @@
         <v>49</v>
       </c>
       <c r="D80" s="26" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E80" s="27" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="F80" s="28"/>
       <c r="G80" s="29"/>
@@ -5752,7 +5776,7 @@
       <c r="R80" s="31"/>
       <c r="S80" s="32"/>
       <c r="T80" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5766,10 +5790,10 @@
         <v>49</v>
       </c>
       <c r="D81" s="26" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E81" s="27" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F81" s="28"/>
       <c r="G81" s="29"/>
@@ -5779,7 +5803,7 @@
         <v>55</v>
       </c>
       <c r="K81" s="30" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="L81" s="30"/>
       <c r="M81" s="30"/>
@@ -5790,7 +5814,7 @@
       <c r="R81" s="31"/>
       <c r="S81" s="32"/>
       <c r="T81" s="33" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12272,25 +12296,25 @@
         <v>49</v>
       </c>
       <c r="D376" s="26" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E376" s="27" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F376" s="28" t="n">
         <v>45320</v>
       </c>
       <c r="G376" s="29" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H376" s="29" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="I376" s="29" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="J376" s="30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K376" s="30"/>
       <c r="L376" s="30"/>
@@ -17159,10 +17183,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="B3" activeCellId="1" sqref="J15:J376 B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.88"/>
@@ -17179,24 +17203,24 @@
         <v>29</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17204,125 +17228,125 @@
         <v>49</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D3" s="36" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D5" s="36" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C6" s="36" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C7" s="36" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C8" s="36" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C11" s="36" t="n">
         <v>192</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17330,111 +17354,111 @@
         <v>49</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C12" s="36" t="n">
         <v>208</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C13" s="36" t="n">
         <v>224</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C14" s="36" t="n">
         <v>240</v>
       </c>
       <c r="D14" s="36" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C15" s="36" t="n">
         <v>256</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C16" s="36" t="n">
         <v>272</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C17" s="36" t="n">
         <v>288</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C18" s="36" t="n">
         <v>304</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C19" s="36" t="n">
         <v>193</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17442,111 +17466,111 @@
         <v>49</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C20" s="36" t="n">
         <v>209</v>
       </c>
       <c r="D20" s="36" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C21" s="36" t="n">
         <v>225</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C22" s="36" t="n">
         <v>241</v>
       </c>
       <c r="D22" s="36" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C23" s="36" t="n">
         <v>257</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C24" s="36" t="n">
         <v>273</v>
       </c>
       <c r="D24" s="37" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C25" s="36" t="n">
         <v>289</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C26" s="36" t="n">
         <v>305</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C27" s="36" t="n">
         <v>194</v>
       </c>
       <c r="D27" s="36" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17554,105 +17578,105 @@
         <v>49</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C28" s="36" t="n">
         <v>210</v>
       </c>
       <c r="D28" s="36" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C29" s="36" t="n">
         <v>226</v>
       </c>
       <c r="D29" s="38" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C30" s="36" t="n">
         <v>242</v>
       </c>
       <c r="D30" s="36" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C31" s="36" t="n">
         <v>258</v>
       </c>
       <c r="D31" s="37" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C32" s="36" t="n">
         <v>274</v>
       </c>
       <c r="D32" s="37" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C33" s="36" t="n">
         <v>290</v>
       </c>
       <c r="D33" s="37" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="10" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C34" s="36" t="n">
         <v>306</v>
       </c>
       <c r="D34" s="37" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C35" s="36" t="n">
         <v>195</v>
@@ -17666,7 +17690,7 @@
         <v>49</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C36" s="36" t="n">
         <v>211</v>
@@ -17677,10 +17701,10 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C37" s="36" t="n">
         <v>227</v>
@@ -17691,10 +17715,10 @@
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C38" s="36" t="n">
         <v>243</v>
@@ -17705,10 +17729,10 @@
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C39" s="36" t="n">
         <v>259</v>
@@ -17719,10 +17743,10 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C40" s="36" t="n">
         <v>275</v>
@@ -17733,10 +17757,10 @@
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C41" s="36" t="n">
         <v>291</v>
@@ -17747,10 +17771,10 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="10" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C42" s="36" t="n">
         <v>307</v>
@@ -17761,10 +17785,10 @@
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="10" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C43" s="36" t="n">
         <v>196</v>
@@ -17778,7 +17802,7 @@
         <v>49</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C44" s="36" t="n">
         <v>212</v>
@@ -17789,10 +17813,10 @@
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B45" s="10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C45" s="36" t="n">
         <v>228</v>
@@ -17803,10 +17827,10 @@
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C46" s="36" t="n">
         <v>244</v>
@@ -17817,10 +17841,10 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C47" s="36" t="n">
         <v>260</v>
@@ -17831,10 +17855,10 @@
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C48" s="36" t="n">
         <v>276</v>
@@ -17845,10 +17869,10 @@
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C49" s="36" t="n">
         <v>292</v>
@@ -17859,10 +17883,10 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C50" s="36" t="n">
         <v>308</v>
@@ -18840,10 +18864,10 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J15:J376 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.14"/>
@@ -18860,15 +18884,15 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="39" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B2" s="39" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="39" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B3" s="39" t="s">
         <v>55</v>

</xml_diff>